<commit_message>
first working version (needs uc_set testing and some tidying)
</commit_message>
<xml_diff>
--- a/PREPARE-TIMES-NZ/output/SysSettings.xlsx
+++ b/PREPARE-TIMES-NZ/output/SysSettings.xlsx
@@ -415,14 +415,306 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>~StartYear</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>~ActivePDef</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>5Year_increments</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>~TimePeriods</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>5Year_increments</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1Year_increments</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>5</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>5</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>5</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>~BookRegions_Map</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>BookName</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>TIMES_NZ</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NI</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>~Currencies</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>MioNZDollar</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -433,14 +725,92 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>~TimeSlices</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Season</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DayNite</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SUM-</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>WK-</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FAL-</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>WE-</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WIN-</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SPR-</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -451,14 +821,447 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>~YRFR</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TimeSlice</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Attribute</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>AllRegions</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SUM-WK-D</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.081</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SUM-WK-N</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.088</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SUM-WK-P</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.007</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SUM-WE-D</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.032</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SUM-WE-N</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.035</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SUM-WE-P</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>FAL-WK-D</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.083</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>FAL-WK-N</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>FAL-WK-P</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.008</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>FAL-WE-D</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>FAL-WE-N</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>FAL-WE-P</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WIN-WK-D</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.083</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WIN-WK-N</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>WIN-WK-P</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.008</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>WIN-WE-D</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>WIN-WE-N</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>WIN-WE-P</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SPR-WK-D</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.082</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SPR-WK-N</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.089</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>SPR-WK-P</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0.007</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>SPR-WE-D</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>SPR-WE-N</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.0339999999999999</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>SPR-WE-P</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>YRFR</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>